<commit_message>
sample code for client
</commit_message>
<xml_diff>
--- a/docs/paths.xlsx
+++ b/docs/paths.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="API" sheetId="1" r:id="rId1"/>
-    <sheet name="Routes" sheetId="2" r:id="rId2"/>
+    <sheet name="Server API" sheetId="1" r:id="rId1"/>
+    <sheet name="Client Routes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Data</t>
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>Parameters</t>
   </si>
   <si>
     <t>Category List</t>
@@ -258,13 +255,37 @@
   </si>
   <si>
     <t>search.client.view.html</t>
+  </si>
+  <si>
+    <t>Session parameters</t>
+  </si>
+  <si>
+    <t>Query Parameters</t>
+  </si>
+  <si>
+    <t>cityID</t>
+  </si>
+  <si>
+    <t>Controller function</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +297,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -312,6 +348,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -594,179 +636,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" style="3" customWidth="1"/>
-    <col min="3" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="L13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="I16" t="s">
         <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -781,15 +859,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="33" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -797,186 +875,187 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
+      <c r="C2" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>